<commit_message>
Added data for method 2
</commit_message>
<xml_diff>
--- a/Alldata.xlsx
+++ b/Alldata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\OneDrive - ICIMOD\15 Feb 2022\2. GMBA\3A. Interactions\SDGIntearctions_Nepal_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9998271-C395-4022-BEC1-969FA55B79B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CC9BEF-3AF3-4C54-876E-C2886C4EFA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{62811C61-2319-451F-B6CB-095D1B0878FF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{62811C61-2319-451F-B6CB-095D1B0878FF}"/>
   </bookViews>
   <sheets>
     <sheet name="method1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="255">
   <si>
     <t>institution</t>
   </si>
@@ -726,13 +726,79 @@
   </si>
   <si>
     <t>Mountain areas are fragile and need careful development interventions</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>forest_cover</t>
+  </si>
+  <si>
+    <t>kba_freshwater</t>
+  </si>
+  <si>
+    <t>kba_terrestrial</t>
+  </si>
+  <si>
+    <t>redlist</t>
+  </si>
+  <si>
+    <t>undernourishment</t>
+  </si>
+  <si>
+    <t>food_insecurity</t>
+  </si>
+  <si>
+    <t>death_chronic</t>
+  </si>
+  <si>
+    <t>suicide</t>
+  </si>
+  <si>
+    <t>uhc_index</t>
+  </si>
+  <si>
+    <t>f_parliament</t>
+  </si>
+  <si>
+    <t>safewater</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>cleanfuel</t>
+  </si>
+  <si>
+    <t>renewable</t>
+  </si>
+  <si>
+    <t>gdp_capita</t>
+  </si>
+  <si>
+    <t>manu_value</t>
+  </si>
+  <si>
+    <t>consumption_gdp</t>
+  </si>
+  <si>
+    <t>consumption_all</t>
+  </si>
+  <si>
+    <t>consumption_cap</t>
+  </si>
+  <si>
+    <t>death_missing</t>
+  </si>
+  <si>
+    <t>local_drr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -740,16 +806,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -757,12 +835,207 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9825,12 +10098,1632 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B184FBD-B235-4698-9D4B-09B51F546AF6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:V33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
+        <v>1990</v>
+      </c>
+      <c r="B2" s="9">
+        <v>0.39664335664335704</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="14"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.39740391608391595</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="14"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.39816447552447498</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="14"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.39892503496503501</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="15">
+        <v>0.82532000000000005</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="14"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.39968559440559404</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="15">
+        <v>0.82516999999999996</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="14"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.40044615384615395</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="15">
+        <v>0.82509999999999994</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="14"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.40120671328671298</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="15">
+        <v>0.82460999999999995</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="9">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="N8" s="13"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="14"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.40196727272727301</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="15">
+        <v>0.82445000000000002</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="9">
+        <v>0.15564610000000001</v>
+      </c>
+      <c r="N9" s="13"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="14"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0.40272783216783203</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="15">
+        <v>0.82426999999999995</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="9">
+        <v>0.19429279999999999</v>
+      </c>
+      <c r="N10" s="13"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="14"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.40348839160839201</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="15">
+        <v>0.82393000000000005</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="9">
+        <v>0.2329445</v>
+      </c>
+      <c r="N11" s="13"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="14"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0.41651621904429703</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0.2496921</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0.39234859999999999</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.83521000000000001</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="13">
+        <v>27.3</v>
+      </c>
+      <c r="I12" s="13">
+        <v>8.5</v>
+      </c>
+      <c r="J12" s="14">
+        <v>24</v>
+      </c>
+      <c r="K12" s="1">
+        <v>5.8536999999999999E-2</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="M12" s="9">
+        <v>0.27155200000000002</v>
+      </c>
+      <c r="N12" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="O12" s="14">
+        <v>0.88290000000000002</v>
+      </c>
+      <c r="P12" s="1">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>8.9099999999999999E-2</v>
+      </c>
+      <c r="R12" s="9">
+        <v>5.6082000000000001</v>
+      </c>
+      <c r="S12" s="13">
+        <v>61703182.558980003</v>
+      </c>
+      <c r="T12" s="13">
+        <v>2.5990199999999999</v>
+      </c>
+      <c r="U12" s="9"/>
+      <c r="V12" s="14"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0.40452647366585304</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0.2496921</v>
+      </c>
+      <c r="D13" s="13">
+        <v>0.39234859999999999</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.83496999999999999</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.22</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="1">
+        <v>5.8536999999999999E-2</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0.24600000000000002</v>
+      </c>
+      <c r="N13" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O13" s="14">
+        <v>0.87760000000000005</v>
+      </c>
+      <c r="P13" s="1">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="R13" s="9">
+        <v>5.8603899999999998</v>
+      </c>
+      <c r="S13" s="13">
+        <v>68107012.551070005</v>
+      </c>
+      <c r="T13" s="13">
+        <v>2.8187899999999999</v>
+      </c>
+      <c r="U13" s="9"/>
+      <c r="V13" s="14"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0.40579100104638999</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.2496921</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0.39926670000000003</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.83477999999999997</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0.214</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="1">
+        <v>5.8536999999999999E-2</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="M14" s="9">
+        <v>0.3484372</v>
+      </c>
+      <c r="N14" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="O14" s="14">
+        <v>0.89939999999999998</v>
+      </c>
+      <c r="P14" s="1">
+        <v>-1.41E-2</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>8.2100000000000006E-2</v>
+      </c>
+      <c r="R14" s="9">
+        <v>6.4254699999999998</v>
+      </c>
+      <c r="S14" s="13">
+        <v>74763615.817900002</v>
+      </c>
+      <c r="T14" s="13">
+        <v>3.0433400000000002</v>
+      </c>
+      <c r="U14" s="9"/>
+      <c r="V14" s="14"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.40705552842692699</v>
+      </c>
+      <c r="C15" s="13">
+        <v>0.2496921</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0.39926670000000003</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.83460999999999996</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0.38661639999999997</v>
+      </c>
+      <c r="N15" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="O15" s="14">
+        <v>0.89439999999999997</v>
+      </c>
+      <c r="P15" s="1">
+        <v>2.4700000000000003E-2</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="R15" s="9">
+        <v>7.0183499999999999</v>
+      </c>
+      <c r="S15" s="13">
+        <v>84883876.612100005</v>
+      </c>
+      <c r="T15" s="13">
+        <v>3.4020700000000001</v>
+      </c>
+      <c r="U15" s="9"/>
+      <c r="V15" s="14"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.408320055807464</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0.31640450000000003</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.42595170000000004</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.83472999999999997</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0.187</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0.37200000000000005</v>
+      </c>
+      <c r="N16" s="13">
+        <v>0.11</v>
+      </c>
+      <c r="O16" s="14">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="P16" s="1">
+        <v>3.2899999999999999E-2</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="R16" s="9">
+        <v>6.5447800000000003</v>
+      </c>
+      <c r="S16" s="13">
+        <v>82862729.852599993</v>
+      </c>
+      <c r="T16" s="13">
+        <v>3.2739799999999999</v>
+      </c>
+      <c r="U16" s="9"/>
+      <c r="V16" s="14"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.40958458318800095</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.31640450000000003</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0.43676589999999998</v>
+      </c>
+      <c r="E17" s="14">
+        <v>0.83440999999999999</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="13">
+        <v>25.8</v>
+      </c>
+      <c r="I17" s="13">
+        <v>7.9</v>
+      </c>
+      <c r="J17" s="14">
+        <v>29</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0.46223219999999998</v>
+      </c>
+      <c r="N17" s="13">
+        <v>0.13</v>
+      </c>
+      <c r="O17" s="14">
+        <v>0.8952</v>
+      </c>
+      <c r="P17" s="1">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>7.6200000000000004E-2</v>
+      </c>
+      <c r="R17" s="9">
+        <v>6.4456600000000002</v>
+      </c>
+      <c r="S17" s="13">
+        <v>84447150.401999995</v>
+      </c>
+      <c r="T17" s="13">
+        <v>3.2935300000000001</v>
+      </c>
+      <c r="U17" s="9">
+        <v>1.77206</v>
+      </c>
+      <c r="V17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.41084911056853896</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0.31640450000000003</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.4723697</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0.83457999999999999</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.16</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="N18" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="O18" s="14">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="P18" s="1">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>7.3099999999999998E-2</v>
+      </c>
+      <c r="R18" s="9">
+        <v>6.2495000000000003</v>
+      </c>
+      <c r="S18" s="13">
+        <v>84631997.908800006</v>
+      </c>
+      <c r="T18" s="13">
+        <v>3.2625299999999999</v>
+      </c>
+      <c r="U18" s="9">
+        <v>2.8263799999999999</v>
+      </c>
+      <c r="V18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.41211363794907596</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.31640450000000003</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.4723697</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0.83453999999999995</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0.152</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="1">
+        <v>0.17325199999999999</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0.53725909999999999</v>
+      </c>
+      <c r="N19" s="13">
+        <v>0.17</v>
+      </c>
+      <c r="O19" s="14">
+        <v>0.91310000000000002</v>
+      </c>
+      <c r="P19" s="1">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>7.17E-2</v>
+      </c>
+      <c r="R19" s="9">
+        <v>6.0192399999999999</v>
+      </c>
+      <c r="S19" s="13">
+        <v>84294623.673999995</v>
+      </c>
+      <c r="T19" s="13">
+        <v>3.2155300000000002</v>
+      </c>
+      <c r="U19" s="9">
+        <v>2.9040400000000002</v>
+      </c>
+      <c r="V19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.41337816532961297</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.31640450000000003</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0.4723697</v>
+      </c>
+      <c r="E20" s="14">
+        <v>0.83442000000000005</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="1">
+        <v>0.17325199999999999</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M20" s="9">
+        <v>0.57487940000000004</v>
+      </c>
+      <c r="N20" s="13">
+        <v>0.18</v>
+      </c>
+      <c r="O20" s="14">
+        <v>0.90469999999999995</v>
+      </c>
+      <c r="P20" s="1">
+        <v>4.9699999999999994E-2</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>7.0099999999999996E-2</v>
+      </c>
+      <c r="R20" s="9">
+        <v>5.8575600000000003</v>
+      </c>
+      <c r="S20" s="13">
+        <v>87038058.211700007</v>
+      </c>
+      <c r="T20" s="13">
+        <v>3.2874500000000002</v>
+      </c>
+      <c r="U20" s="9">
+        <v>4.1699700000000002</v>
+      </c>
+      <c r="V20" s="14">
+        <v>0.503</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0.41464269271014997</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.31640450000000003</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.50334630000000002</v>
+      </c>
+      <c r="E21" s="14">
+        <v>0.83442000000000005</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0.126</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="1">
+        <v>0.33165</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0.61275179999999996</v>
+      </c>
+      <c r="N21" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="O21" s="14">
+        <v>0.88930000000000009</v>
+      </c>
+      <c r="P21" s="1">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>6.6199999999999995E-2</v>
+      </c>
+      <c r="R21" s="9">
+        <v>5.7802100000000003</v>
+      </c>
+      <c r="S21" s="13">
+        <v>89782131.402400002</v>
+      </c>
+      <c r="T21" s="13">
+        <v>3.3574600000000001</v>
+      </c>
+      <c r="U21" s="9">
+        <v>5.4286000000000003</v>
+      </c>
+      <c r="V21" s="14">
+        <v>1.3839999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B22" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0.5065442</v>
+      </c>
+      <c r="E22" s="14">
+        <v>0.83460000000000001</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="13">
+        <v>23.8</v>
+      </c>
+      <c r="I22" s="13">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J22" s="14">
+        <v>42</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.33165</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M22" s="9">
+        <v>0.65101209999999998</v>
+      </c>
+      <c r="N22" s="13">
+        <v>0.21</v>
+      </c>
+      <c r="O22" s="14">
+        <v>0.87290000000000001</v>
+      </c>
+      <c r="P22" s="1">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>5.9500000000000004E-2</v>
+      </c>
+      <c r="R22" s="9">
+        <v>5.6990800000000004</v>
+      </c>
+      <c r="S22" s="13">
+        <v>92785568.874599993</v>
+      </c>
+      <c r="T22" s="13">
+        <v>3.4335599999999999</v>
+      </c>
+      <c r="U22" s="9">
+        <v>4.3765099999999997</v>
+      </c>
+      <c r="V22" s="14">
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.5065442</v>
+      </c>
+      <c r="E23" s="14">
+        <v>0.83433000000000002</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="1">
+        <v>0.33165</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M23" s="9">
+        <v>0.67260000000000009</v>
+      </c>
+      <c r="N23" s="13">
+        <v>0.23</v>
+      </c>
+      <c r="O23" s="14">
+        <v>0.86950000000000005</v>
+      </c>
+      <c r="P23" s="1">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>5.8899999999999994E-2</v>
+      </c>
+      <c r="R23" s="9">
+        <v>5.6283899999999996</v>
+      </c>
+      <c r="S23" s="13">
+        <v>94770229.464900002</v>
+      </c>
+      <c r="T23" s="13">
+        <v>3.4679899999999999</v>
+      </c>
+      <c r="U23" s="9">
+        <v>2.0872299999999999</v>
+      </c>
+      <c r="V23" s="14">
+        <v>8.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C24" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0.5065442</v>
+      </c>
+      <c r="E24" s="14">
+        <v>0.83447000000000005</v>
+      </c>
+      <c r="F24" s="9">
+        <v>9.4E-2</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="1">
+        <v>0.33165</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M24" s="9">
+        <v>0.73873169999999999</v>
+      </c>
+      <c r="N24" s="13">
+        <v>0.24</v>
+      </c>
+      <c r="O24" s="14">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="P24" s="1">
+        <v>4.9800000000000004E-2</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>5.9699999999999996E-2</v>
+      </c>
+      <c r="R24" s="9">
+        <v>5.69069</v>
+      </c>
+      <c r="S24" s="13">
+        <v>100400583.15009999</v>
+      </c>
+      <c r="T24" s="13">
+        <v>3.6311300000000002</v>
+      </c>
+      <c r="U24" s="9">
+        <v>1.83083</v>
+      </c>
+      <c r="V24" s="14">
+        <v>13.465999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C25" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D25" s="13">
+        <v>0.5065442</v>
+      </c>
+      <c r="E25" s="14">
+        <v>0.83467999999999998</v>
+      </c>
+      <c r="F25" s="9">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="1">
+        <v>0.33165</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0.78035700000000008</v>
+      </c>
+      <c r="N25" s="13">
+        <v>0.26</v>
+      </c>
+      <c r="O25" s="14">
+        <v>0.86049999999999993</v>
+      </c>
+      <c r="P25" s="1">
+        <v>4.41E-2</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>5.9200000000000003E-2</v>
+      </c>
+      <c r="R25" s="9">
+        <v>5.4718099999999996</v>
+      </c>
+      <c r="S25" s="13">
+        <v>100524930.48639999</v>
+      </c>
+      <c r="T25" s="13">
+        <v>3.59206</v>
+      </c>
+      <c r="U25" s="9">
+        <v>2.3479899999999998</v>
+      </c>
+      <c r="V25" s="14">
+        <v>18.122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C26" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0.5065442</v>
+      </c>
+      <c r="E26" s="14">
+        <v>0.83450000000000002</v>
+      </c>
+      <c r="F26" s="9">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="1">
+        <v>0.29913000000000001</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="M26" s="9">
+        <v>0.84900000000000009</v>
+      </c>
+      <c r="N26" s="13">
+        <v>0.27</v>
+      </c>
+      <c r="O26" s="14">
+        <v>0.84060000000000001</v>
+      </c>
+      <c r="P26" s="1">
+        <v>6.0299999999999999E-2</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="R26" s="9">
+        <v>5.4128400000000001</v>
+      </c>
+      <c r="S26" s="13">
+        <v>105397062.32179999</v>
+      </c>
+      <c r="T26" s="13">
+        <v>3.7212200000000002</v>
+      </c>
+      <c r="U26" s="9">
+        <v>2.8358500000000002</v>
+      </c>
+      <c r="V26" s="14">
+        <v>22.959</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C27" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0.5065442</v>
+      </c>
+      <c r="E27" s="14">
+        <v>0.83450000000000002</v>
+      </c>
+      <c r="F27" s="9">
+        <v>9.4E-2</v>
+      </c>
+      <c r="G27" s="14">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="H27" s="13">
+        <v>22.2</v>
+      </c>
+      <c r="I27" s="13">
+        <v>8.5</v>
+      </c>
+      <c r="J27" s="14">
+        <v>51</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0.29480699999999999</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0.86655270000000006</v>
+      </c>
+      <c r="N27" s="13">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O27" s="14">
+        <v>0.85040000000000004</v>
+      </c>
+      <c r="P27" s="1">
+        <v>2.9100000000000001E-2</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="R27" s="9">
+        <v>5.3779899999999996</v>
+      </c>
+      <c r="S27" s="13">
+        <v>108198110.83704001</v>
+      </c>
+      <c r="T27" s="13">
+        <v>3.7757200000000002</v>
+      </c>
+      <c r="U27" s="9">
+        <v>33.74004</v>
+      </c>
+      <c r="V27" s="14">
+        <v>23.710999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C28" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0.50657479999999999</v>
+      </c>
+      <c r="E28" s="14">
+        <v>0.83457000000000003</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="14">
+        <v>0.312</v>
+      </c>
+      <c r="H28" s="13">
+        <v>21.8</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="1">
+        <v>0.29549199999999998</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="N28" s="13">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O28" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="P28" s="1">
+        <v>-3.3E-3</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="R28" s="9">
+        <v>5.50868</v>
+      </c>
+      <c r="S28" s="13">
+        <v>111285165.56742001</v>
+      </c>
+      <c r="T28" s="13">
+        <v>3.8397000000000001</v>
+      </c>
+      <c r="U28" s="9">
+        <v>1.7480599999999999</v>
+      </c>
+      <c r="V28" s="14">
+        <v>24.452000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C29" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D29" s="13">
+        <v>0.50657479999999999</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0.83477000000000001</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="14">
+        <v>0.316</v>
+      </c>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14">
+        <v>48</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.29579800000000001</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0.9550748</v>
+      </c>
+      <c r="N29" s="13">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O29" s="14">
+        <v>0.7641</v>
+      </c>
+      <c r="P29" s="1">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>5.0099999999999999E-2</v>
+      </c>
+      <c r="R29" s="9">
+        <v>5.26654</v>
+      </c>
+      <c r="S29" s="13">
+        <v>114372220.2977</v>
+      </c>
+      <c r="T29" s="13">
+        <v>3.9028200000000002</v>
+      </c>
+      <c r="U29" s="9">
+        <v>1.9322999999999999</v>
+      </c>
+      <c r="V29" s="14">
+        <v>1.5940000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B30" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C30" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D30" s="13">
+        <v>0.50657479999999999</v>
+      </c>
+      <c r="E30" s="14">
+        <v>0.83457000000000003</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="14">
+        <v>0.33799999999999997</v>
+      </c>
+      <c r="I30" s="13"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="1">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="M30" s="9"/>
+      <c r="N30" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="O30" s="14">
+        <v>0.75039999999999996</v>
+      </c>
+      <c r="P30" s="1">
+        <v>4.9400000000000006E-2</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>4.99E-2</v>
+      </c>
+      <c r="R30" s="9"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="9">
+        <v>1.66673</v>
+      </c>
+      <c r="V30" s="14">
+        <v>7.4370000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C31" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D31" s="13">
+        <v>0.50657479999999999</v>
+      </c>
+      <c r="E31" s="14">
+        <v>0.83479999999999999</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="14">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="I31" s="13">
+        <v>9</v>
+      </c>
+      <c r="J31" s="16"/>
+      <c r="K31" s="1">
+        <v>0.32727299999999998</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="M31" s="9"/>
+      <c r="N31" s="13">
+        <v>0.31</v>
+      </c>
+      <c r="O31" s="14"/>
+      <c r="P31" s="1">
+        <v>5.0700000000000002E-2</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>4.9800000000000004E-2</v>
+      </c>
+      <c r="R31" s="9"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="9">
+        <v>1.78996</v>
+      </c>
+      <c r="V31" s="14">
+        <v>16.866</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B32" s="9">
+        <v>0.41590722009068698</v>
+      </c>
+      <c r="C32" s="13">
+        <v>0.32431699999999997</v>
+      </c>
+      <c r="D32" s="13">
+        <v>0.50657479999999999</v>
+      </c>
+      <c r="E32" s="14">
+        <v>0.83479999999999999</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="1">
+        <v>0.32727299999999998</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="M32" s="9"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="14"/>
+    </row>
+    <row r="33" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="19">
+        <v>2021</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="22">
+        <v>0.83470999999999995</v>
+      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="19">
+        <v>0.32727299999999998</v>
+      </c>
+      <c r="L33" s="24"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="25"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="25"/>
+      <c r="V33" s="22"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9839,7 +11732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F01EF7D-A732-4A56-9814-4C64AF3D13DE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>

</xml_diff>